<commit_message>
Code giao diện hiển thị vật liệu ở trang giao dịch
</commit_message>
<xml_diff>
--- a/QuanLyCuaHangVatLieuXayDung/template/layout.xlsx
+++ b/QuanLyCuaHangVatLieuXayDung/template/layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Phan_Tich_Va_Thiet_Ke_He_Thong_Thong_Tin\DoAnCuoiKy\QuanLyNhapXuatCuaHangVatLieuXayDung_dev_Bao\QuanLyCuaHangVatLieuXayDung\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E123ED-ECD6-4BD9-A22C-CB1E8FB859EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E837C6B-5479-42EA-8D94-7909A456AEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{30F8D3DC-B8FB-4EF1-8873-75A4B0B7C454}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>Tên: Gạch 2 lổ TCVN</t>
   </si>
@@ -86,7 +86,67 @@
     <t>Đăng xuất</t>
   </si>
   <si>
-    <t>Gía nhập: 990 đ/viên</t>
+    <t>Hoa Đơn Xuất</t>
+  </si>
+  <si>
+    <t>Ngày: 7/4/2025</t>
+  </si>
+  <si>
+    <t>Tên khách hàng:</t>
+  </si>
+  <si>
+    <t>SĐT:</t>
+  </si>
+  <si>
+    <t>Địa chỉ:</t>
+  </si>
+  <si>
+    <t>Stt</t>
+  </si>
+  <si>
+    <t>Mã</t>
+  </si>
+  <si>
+    <t>Tên</t>
+  </si>
+  <si>
+    <t>Gía</t>
+  </si>
+  <si>
+    <t>Đơn vị</t>
+  </si>
+  <si>
+    <t>Số lượng</t>
+  </si>
+  <si>
+    <t>Tổng tiền</t>
+  </si>
+  <si>
+    <t>Phương thức thanh toán:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Số tiền thanh toán: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiền giảm: </t>
+  </si>
+  <si>
+    <t>Nợ củ</t>
+  </si>
+  <si>
+    <t>Tổng hóa đơn:</t>
+  </si>
+  <si>
+    <t>Xuất hóa đơn</t>
+  </si>
+  <si>
+    <t>Mã: VatLieu001</t>
+  </si>
+  <si>
+    <t>Mã hóa đơn:</t>
+  </si>
+  <si>
+    <t>Hd00000001</t>
   </si>
 </sst>
 </file>
@@ -114,20 +174,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="24"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <i/>
-      <u/>
-      <sz val="22"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="22"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -146,8 +192,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,8 +245,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -335,38 +414,114 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -385,29 +540,108 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -420,103 +654,96 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -854,86 +1081,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>59764</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>134471</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>538949</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>37353</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Oval 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E779A8D-28D0-8E0C-94E1-A9D76F18F459}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12468411" y="13155706"/>
-          <a:ext cx="479185" cy="478118"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FF0000"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="4000">
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t>+</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>12391</xdr:rowOff>
+      <xdr:colOff>206375</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>22087</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>216829</xdr:colOff>
+      <xdr:colOff>220869</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>186531</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -948,8 +1105,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="4639062" y="2902415"/>
-          <a:ext cx="7279" cy="293958"/>
+          <a:off x="4643438" y="3070087"/>
+          <a:ext cx="14494" cy="164444"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1041,13 +1198,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>194469</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:colOff>193260</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>22087</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>196850</xdr:colOff>
+      <xdr:colOff>194469</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
@@ -1063,9 +1220,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="1416844" y="2909094"/>
-          <a:ext cx="2381" cy="317500"/>
+        <a:xfrm>
+          <a:off x="1408043" y="3092174"/>
+          <a:ext cx="1209" cy="136663"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1443,13 +1600,13 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>21896</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>87587</xdr:rowOff>
+      <xdr:rowOff>65176</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>21896</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>67236</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>109483</xdr:rowOff>
+      <xdr:rowOff>119529</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1464,8 +1621,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7484241" y="5399690"/>
-          <a:ext cx="4261069" cy="214586"/>
+          <a:off x="7529837" y="5429058"/>
+          <a:ext cx="3108281" cy="248589"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1530,16 +1687,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>175172</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>249879</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>87587</xdr:rowOff>
+      <xdr:rowOff>80116</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>407276</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>481982</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>113862</xdr:rowOff>
+      <xdr:rowOff>106391</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1554,8 +1711,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11898586" y="5399690"/>
-          <a:ext cx="840828" cy="218965"/>
+          <a:off x="10820761" y="5443998"/>
+          <a:ext cx="844692" cy="220511"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1600,6 +1757,628 @@
             <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>48172</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>80117</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>530412</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104589</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectangle 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{577C87AF-BA13-22C5-AE97-5A05F807F957}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11844231" y="5443999"/>
+          <a:ext cx="1094828" cy="218708"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Tạo</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> hóa đơn</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1300">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>44174</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>16565</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>375477</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>55217</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97C4EBEA-6406-EB6A-4613-9F16794740EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11744739" y="6758608"/>
+          <a:ext cx="938695" cy="463826"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Chọn</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>đối</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> tác</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1300">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>49696</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>204303</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>392043</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>93869</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8501B6B5-E68E-B54B-5DC9-5CA8CFF4D9BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11750261" y="7371520"/>
+          <a:ext cx="949739" cy="519045"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Tạo</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> đối tác mới</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>53009</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>180008</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>384312</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>47487</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02A00C59-559C-730C-A1DA-4799368F31B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11764618" y="8169965"/>
+          <a:ext cx="1093303" cy="463826"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Chọn</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>vật liệu</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1300">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>58531</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>3312</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>400878</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>146879</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectangle 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D52A255D-9F9E-3AF4-E840-DAFD63CC16CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11770140" y="8782877"/>
+          <a:ext cx="1104347" cy="519045"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Tạo</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> vật liệu mới</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>320261</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>121479</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>27608</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>66262</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Graphic 14" descr="Caret Down outline">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02D85096-40FD-8108-160B-D7AC471C481F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId6"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10198652" y="11176001"/>
+          <a:ext cx="314739" cy="342348"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Rectangle 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A77D106-5861-45ED-926B-1E6EE9671C4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="620091" y="218661"/>
+          <a:ext cx="1786283" cy="1061830"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill dpi="0" rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+              <a:alpha val="98000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Rectangle 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7CB95B-BEA3-4654-9CE2-90AD0399D3C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="622300" y="215900"/>
+          <a:ext cx="1790700" cy="1066800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:blipFill dpi="0" rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </a:blipFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+              <a:alpha val="98000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1927,192 +2706,206 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A237127A-16A2-4193-9CBC-875260166E60}">
   <dimension ref="B1:V72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AB41" sqref="AB41"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U34" sqref="U34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="5" max="5" width="2.26953125" customWidth="1"/>
+    <col min="20" max="20" width="8.81640625" customWidth="1"/>
+    <col min="21" max="21" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="15"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="17"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="9"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="20"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="12"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="20"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="12"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="20"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="12"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="20"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="12"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B7" s="21"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="23"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="23"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="15"/>
     </row>
     <row r="8" spans="2:10" ht="22" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="18"/>
+      <c r="H8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="J8" s="18"/>
+    </row>
+    <row r="9" spans="2:10" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="26"/>
-      <c r="H8" s="24" t="s">
+      <c r="C9" s="17"/>
+      <c r="D9" s="18"/>
+      <c r="H9" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="I8" s="25"/>
-      <c r="J8" s="26"/>
-    </row>
-    <row r="9" spans="2:10" ht="22" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="24" t="s">
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
+    </row>
+    <row r="10" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="26"/>
-      <c r="H9" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="25"/>
-      <c r="J9" s="26"/>
-    </row>
-    <row r="10" spans="2:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="24" t="s">
+      <c r="C10" s="17"/>
+      <c r="D10" s="18"/>
+      <c r="H10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18"/>
+    </row>
+    <row r="11" spans="2:10" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="26"/>
-      <c r="H10" s="24" t="s">
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
+      <c r="H11" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="I10" s="25"/>
-      <c r="J10" s="26"/>
-    </row>
-    <row r="11" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="27" t="s">
+      <c r="I11" s="17"/>
+      <c r="J11" s="18"/>
+    </row>
+    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="29"/>
-      <c r="H11" s="27" t="s">
+      <c r="C12" s="97"/>
+      <c r="D12" s="98"/>
+      <c r="H12" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="I11" s="28"/>
-      <c r="J11" s="29"/>
-    </row>
-    <row r="12" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="30"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="32"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="32"/>
-    </row>
-    <row r="13" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="9" t="s">
+      <c r="I12" s="97"/>
+      <c r="J12" s="98"/>
+    </row>
+    <row r="13" spans="2:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="99"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="98"/>
+      <c r="H13" s="99"/>
+      <c r="I13" s="97"/>
+      <c r="J13" s="98"/>
+    </row>
+    <row r="14" spans="2:10" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="H13" s="9" t="s">
+      <c r="C14" s="100"/>
+      <c r="D14" s="101"/>
+      <c r="H14" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="10"/>
-      <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="14"/>
-    </row>
-    <row r="15" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+      <c r="I14" s="100"/>
+      <c r="J14" s="101"/>
+    </row>
+    <row r="15" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="102"/>
+      <c r="C15" s="103"/>
+      <c r="D15" s="104"/>
+      <c r="H15" s="102"/>
+      <c r="I15" s="103"/>
+      <c r="J15" s="104"/>
+    </row>
+    <row r="16" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="28" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="42"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="44"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
-      <c r="Q28" s="2"/>
-      <c r="R28" s="2"/>
-      <c r="S28" s="2"/>
-      <c r="T28" s="2"/>
-      <c r="U28" s="2"/>
-      <c r="V28" s="3"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="58"/>
+      <c r="I28" s="58"/>
+      <c r="J28" s="58"/>
+      <c r="K28" s="58"/>
+      <c r="L28" s="58"/>
+      <c r="M28" s="61"/>
+      <c r="N28" s="61"/>
+      <c r="O28" s="61"/>
+      <c r="P28" s="61"/>
+      <c r="Q28" s="61"/>
+      <c r="R28" s="61"/>
+      <c r="S28" s="61"/>
+      <c r="T28" s="61"/>
+      <c r="U28" s="61"/>
+      <c r="V28" s="62"/>
     </row>
     <row r="29" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="45"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="41"/>
-      <c r="M29" s="36"/>
-      <c r="N29" s="36"/>
-      <c r="O29" s="36"/>
-      <c r="P29" s="36"/>
-      <c r="Q29" s="36"/>
-      <c r="R29" s="36"/>
-      <c r="S29" s="36"/>
-      <c r="T29" s="36"/>
-      <c r="U29" s="36"/>
-      <c r="V29" s="37"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="60"/>
+      <c r="K29" s="60"/>
+      <c r="L29" s="60"/>
+      <c r="M29" s="46"/>
+      <c r="N29" s="46"/>
+      <c r="O29" s="46"/>
+      <c r="P29" s="46"/>
+      <c r="Q29" s="46"/>
+      <c r="R29" s="46"/>
+      <c r="S29" s="46"/>
+      <c r="T29" s="46"/>
+      <c r="U29" s="46"/>
+      <c r="V29" s="47"/>
     </row>
     <row r="30" spans="2:22" ht="6.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="45"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="46"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="41"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -2121,386 +2914,413 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-      <c r="U30" s="1"/>
-      <c r="V30" s="34"/>
+      <c r="M30" s="68" t="s">
+        <v>16</v>
+      </c>
+      <c r="N30" s="69"/>
+      <c r="O30" s="69"/>
+      <c r="P30" s="69"/>
+      <c r="Q30" s="69"/>
+      <c r="R30" s="69"/>
+      <c r="S30" s="69"/>
+      <c r="T30" s="69"/>
+      <c r="U30" s="69"/>
+      <c r="V30" s="70"/>
     </row>
     <row r="31" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="4"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="5"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="44"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="17"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="9"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="1"/>
-      <c r="T31" s="1"/>
-      <c r="U31" s="1"/>
-      <c r="V31" s="34"/>
+      <c r="M31" s="71"/>
+      <c r="N31" s="72"/>
+      <c r="O31" s="72"/>
+      <c r="P31" s="72"/>
+      <c r="Q31" s="72"/>
+      <c r="R31" s="72"/>
+      <c r="S31" s="72"/>
+      <c r="T31" s="72"/>
+      <c r="U31" s="72"/>
+      <c r="V31" s="73"/>
     </row>
     <row r="32" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="35"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="37"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="47"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="20"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="12"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
-      <c r="S32" s="1"/>
-      <c r="T32" s="1"/>
-      <c r="U32" s="1"/>
-      <c r="V32" s="34"/>
+      <c r="M32" s="71"/>
+      <c r="N32" s="72"/>
+      <c r="O32" s="72"/>
+      <c r="P32" s="72"/>
+      <c r="Q32" s="72"/>
+      <c r="R32" s="72"/>
+      <c r="S32" s="72"/>
+      <c r="T32" s="72"/>
+      <c r="U32" s="72"/>
+      <c r="V32" s="73"/>
     </row>
     <row r="33" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="66" t="s">
+      <c r="B33" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="67"/>
-      <c r="D33" s="68"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="50"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="20"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="12"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
-      <c r="T33" s="1"/>
-      <c r="U33" s="1"/>
-      <c r="V33" s="34"/>
-    </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B34" s="69"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="71"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="63"/>
+      <c r="O33" s="63"/>
+      <c r="P33" s="63"/>
+      <c r="Q33" s="63"/>
+      <c r="R33" s="63"/>
+      <c r="S33" s="63"/>
+      <c r="T33" s="63"/>
+      <c r="U33" s="63"/>
+      <c r="V33" s="6"/>
+    </row>
+    <row r="34" spans="2:22" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B34" s="51"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="53"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="20"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="12"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
-      <c r="S34" s="1"/>
-      <c r="T34" s="1"/>
-      <c r="U34" s="1"/>
-      <c r="V34" s="34"/>
+      <c r="M34" s="74" t="s">
+        <v>35</v>
+      </c>
+      <c r="N34" s="67"/>
+      <c r="O34" s="108" t="s">
+        <v>36</v>
+      </c>
+      <c r="P34" s="89"/>
+      <c r="Q34" s="107"/>
+      <c r="R34" s="75" t="s">
+        <v>17</v>
+      </c>
+      <c r="S34" s="67"/>
+      <c r="T34" s="107"/>
+      <c r="U34" s="63"/>
+      <c r="V34" s="6"/>
     </row>
     <row r="35" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="72"/>
-      <c r="C35" s="73"/>
-      <c r="D35" s="74"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="55"/>
+      <c r="D35" s="56"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="20"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="12"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
-      <c r="R35" s="1"/>
-      <c r="S35" s="1"/>
-      <c r="T35" s="1"/>
-      <c r="U35" s="1"/>
-      <c r="V35" s="34"/>
-    </row>
-    <row r="36" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="57" t="s">
+      <c r="M35" s="5"/>
+      <c r="N35" s="63"/>
+      <c r="O35" s="63"/>
+      <c r="P35" s="63"/>
+      <c r="Q35" s="63"/>
+      <c r="R35" s="63"/>
+      <c r="S35" s="63"/>
+      <c r="T35" s="63"/>
+      <c r="U35" s="63"/>
+      <c r="V35" s="6"/>
+    </row>
+    <row r="36" spans="2:22" ht="17" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="49"/>
-      <c r="D36" s="50"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="21"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="23"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="15"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
-      <c r="Q36" s="1"/>
-      <c r="R36" s="1"/>
-      <c r="S36" s="1"/>
-      <c r="T36" s="1"/>
-      <c r="U36" s="1"/>
-      <c r="V36" s="34"/>
+      <c r="M36" s="76" t="s">
+        <v>18</v>
+      </c>
+      <c r="N36" s="77"/>
+      <c r="O36" s="80"/>
+      <c r="P36" s="67"/>
+      <c r="Q36" s="67"/>
+      <c r="R36" s="67"/>
+      <c r="S36" s="67"/>
+      <c r="T36" s="63"/>
+      <c r="U36" s="63"/>
+      <c r="V36" s="6"/>
     </row>
     <row r="37" spans="2:22" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B37" s="51"/>
-      <c r="C37" s="52"/>
-      <c r="D37" s="53"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="24"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="G37" s="25"/>
-      <c r="H37" s="26"/>
+      <c r="F37" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G37" s="17"/>
+      <c r="H37" s="18"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
-      <c r="S37" s="1"/>
-      <c r="T37" s="1"/>
-      <c r="U37" s="1"/>
-      <c r="V37" s="34"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="63"/>
+      <c r="O37" s="63"/>
+      <c r="P37" s="63"/>
+      <c r="Q37" s="63"/>
+      <c r="R37" s="63"/>
+      <c r="S37" s="63"/>
+      <c r="T37" s="63"/>
+      <c r="U37" s="63"/>
+      <c r="V37" s="6"/>
     </row>
     <row r="38" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="54"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="56"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="27"/>
       <c r="E38" s="1"/>
-      <c r="F38" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="G38" s="25"/>
-      <c r="H38" s="26"/>
+      <c r="F38" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G38" s="17"/>
+      <c r="H38" s="18"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
-      <c r="S38" s="1"/>
-      <c r="T38" s="1"/>
-      <c r="U38" s="1"/>
-      <c r="V38" s="34"/>
-    </row>
-    <row r="39" spans="2:22" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="57" t="s">
+      <c r="M38" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="N38" s="79"/>
+      <c r="O38" s="80"/>
+      <c r="P38" s="81"/>
+      <c r="Q38" s="81"/>
+      <c r="R38" s="81"/>
+      <c r="S38" s="81"/>
+      <c r="T38" s="63"/>
+      <c r="U38" s="63"/>
+      <c r="V38" s="6"/>
+    </row>
+    <row r="39" spans="2:22" ht="17" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="49"/>
-      <c r="D39" s="50"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="21"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="G39" s="25"/>
-      <c r="H39" s="26"/>
+      <c r="F39" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" s="17"/>
+      <c r="H39" s="18"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
-      <c r="P39" s="1"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
-      <c r="S39" s="1"/>
-      <c r="T39" s="1"/>
-      <c r="U39" s="1"/>
-      <c r="V39" s="34"/>
-    </row>
-    <row r="40" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="51"/>
-      <c r="C40" s="52"/>
-      <c r="D40" s="53"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="63"/>
+      <c r="O39" s="63"/>
+      <c r="P39" s="63"/>
+      <c r="Q39" s="63"/>
+      <c r="R39" s="63"/>
+      <c r="S39" s="63"/>
+      <c r="T39" s="63"/>
+      <c r="U39" s="63"/>
+      <c r="V39" s="6"/>
+    </row>
+    <row r="40" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="22"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="24"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G40" s="28"/>
-      <c r="H40" s="29"/>
+      <c r="F40" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G40" s="17"/>
+      <c r="H40" s="18"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
-      <c r="S40" s="1"/>
-      <c r="T40" s="1"/>
-      <c r="U40" s="1"/>
-      <c r="V40" s="34"/>
-    </row>
-    <row r="41" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="54"/>
-      <c r="C41" s="55"/>
-      <c r="D41" s="56"/>
+      <c r="M40" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N40" s="63"/>
+      <c r="O40" s="80"/>
+      <c r="P40" s="81"/>
+      <c r="Q40" s="81"/>
+      <c r="R40" s="81"/>
+      <c r="S40" s="81"/>
+      <c r="T40" s="63"/>
+      <c r="U40" s="63"/>
+      <c r="V40" s="6"/>
+    </row>
+    <row r="41" spans="2:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B41" s="25"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="27"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="32"/>
+      <c r="F41" s="105" t="s">
+        <v>2</v>
+      </c>
+      <c r="G41" s="97"/>
+      <c r="H41" s="98"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
-      <c r="R41" s="1"/>
-      <c r="S41" s="1"/>
-      <c r="T41" s="1"/>
-      <c r="U41" s="1"/>
-      <c r="V41" s="34"/>
-    </row>
-    <row r="42" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="57" t="s">
+      <c r="M41" s="5"/>
+      <c r="N41" s="63"/>
+      <c r="O41" s="81"/>
+      <c r="P41" s="81"/>
+      <c r="Q41" s="81"/>
+      <c r="R41" s="81"/>
+      <c r="S41" s="81"/>
+      <c r="T41" s="63"/>
+      <c r="U41" s="63"/>
+      <c r="V41" s="6"/>
+    </row>
+    <row r="42" spans="2:22" ht="15.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B42" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="58"/>
-      <c r="D42" s="59"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="29"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G42" s="10"/>
-      <c r="H42" s="11"/>
+      <c r="F42" s="99"/>
+      <c r="G42" s="97"/>
+      <c r="H42" s="98"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
-      <c r="P42" s="1"/>
-      <c r="Q42" s="1"/>
-      <c r="R42" s="1"/>
-      <c r="S42" s="1"/>
-      <c r="T42" s="1"/>
-      <c r="U42" s="1"/>
-      <c r="V42" s="34"/>
-    </row>
-    <row r="43" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="60"/>
-      <c r="C43" s="61"/>
-      <c r="D43" s="62"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="63"/>
+      <c r="O42" s="63"/>
+      <c r="P42" s="63"/>
+      <c r="Q42" s="63"/>
+      <c r="R42" s="63"/>
+      <c r="S42" s="63"/>
+      <c r="T42" s="63"/>
+      <c r="U42" s="63"/>
+      <c r="V42" s="6"/>
+    </row>
+    <row r="43" spans="2:22" ht="15.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B43" s="30"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="32"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="14"/>
+      <c r="F43" s="106" t="s">
+        <v>3</v>
+      </c>
+      <c r="G43" s="100"/>
+      <c r="H43" s="101"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="1"/>
-      <c r="R43" s="1"/>
-      <c r="S43" s="1"/>
-      <c r="T43" s="1"/>
-      <c r="U43" s="1"/>
-      <c r="V43" s="34"/>
+      <c r="M43" s="84" t="s">
+        <v>21</v>
+      </c>
+      <c r="N43" s="84" t="s">
+        <v>22</v>
+      </c>
+      <c r="O43" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="P43" s="84" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q43" s="84" t="s">
+        <v>25</v>
+      </c>
+      <c r="R43" s="84" t="s">
+        <v>26</v>
+      </c>
+      <c r="S43" s="84" t="s">
+        <v>27</v>
+      </c>
+      <c r="T43" s="63"/>
+      <c r="U43" s="63"/>
+      <c r="V43" s="6"/>
     </row>
     <row r="44" spans="2:22" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="63"/>
-      <c r="C44" s="64"/>
-      <c r="D44" s="65"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="35"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
+      <c r="F44" s="102"/>
+      <c r="G44" s="103"/>
+      <c r="H44" s="104"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
-      <c r="Q44" s="1"/>
-      <c r="R44" s="1"/>
-      <c r="S44" s="1"/>
-      <c r="T44" s="1"/>
-      <c r="U44" s="1"/>
-      <c r="V44" s="34"/>
+      <c r="M44" s="82"/>
+      <c r="N44" s="83"/>
+      <c r="O44" s="83"/>
+      <c r="P44" s="83"/>
+      <c r="Q44" s="83"/>
+      <c r="R44" s="83"/>
+      <c r="S44" s="83"/>
+      <c r="T44" s="63"/>
+      <c r="U44" s="63"/>
+      <c r="V44" s="6"/>
     </row>
     <row r="45" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="57" t="s">
+      <c r="B45" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C45" s="49"/>
-      <c r="D45" s="50"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="21"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
-      <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
-      <c r="Q45" s="1"/>
-      <c r="R45" s="1"/>
-      <c r="S45" s="1"/>
-      <c r="T45" s="1"/>
-      <c r="U45" s="1"/>
-      <c r="V45" s="34"/>
+      <c r="M45" s="82"/>
+      <c r="N45" s="83"/>
+      <c r="O45" s="83"/>
+      <c r="P45" s="83"/>
+      <c r="Q45" s="83"/>
+      <c r="R45" s="83"/>
+      <c r="S45" s="83"/>
+      <c r="T45" s="63"/>
+      <c r="U45" s="63"/>
+      <c r="V45" s="6"/>
     </row>
     <row r="46" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B46" s="51"/>
-      <c r="C46" s="52"/>
-      <c r="D46" s="53"/>
+      <c r="B46" s="22"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="24"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -2509,21 +3329,21 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
-      <c r="P46" s="1"/>
-      <c r="Q46" s="1"/>
-      <c r="R46" s="1"/>
-      <c r="S46" s="1"/>
-      <c r="T46" s="1"/>
-      <c r="U46" s="1"/>
-      <c r="V46" s="34"/>
+      <c r="M46" s="82"/>
+      <c r="N46" s="83"/>
+      <c r="O46" s="83"/>
+      <c r="P46" s="83"/>
+      <c r="Q46" s="83"/>
+      <c r="R46" s="83"/>
+      <c r="S46" s="83"/>
+      <c r="T46" s="63"/>
+      <c r="U46" s="63"/>
+      <c r="V46" s="6"/>
     </row>
     <row r="47" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="54"/>
-      <c r="C47" s="55"/>
-      <c r="D47" s="56"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="27"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -2532,23 +3352,23 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
-      <c r="Q47" s="1"/>
-      <c r="R47" s="1"/>
-      <c r="S47" s="1"/>
-      <c r="T47" s="1"/>
-      <c r="U47" s="1"/>
-      <c r="V47" s="34"/>
+      <c r="M47" s="82"/>
+      <c r="N47" s="83"/>
+      <c r="O47" s="83"/>
+      <c r="P47" s="83"/>
+      <c r="Q47" s="83"/>
+      <c r="R47" s="83"/>
+      <c r="S47" s="83"/>
+      <c r="T47" s="63"/>
+      <c r="U47" s="63"/>
+      <c r="V47" s="6"/>
     </row>
     <row r="48" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="57" t="s">
+      <c r="B48" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C48" s="49"/>
-      <c r="D48" s="50"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="21"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -2557,21 +3377,21 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
-      <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
-      <c r="Q48" s="1"/>
-      <c r="R48" s="1"/>
-      <c r="S48" s="1"/>
-      <c r="T48" s="1"/>
-      <c r="U48" s="1"/>
-      <c r="V48" s="34"/>
+      <c r="M48" s="82"/>
+      <c r="N48" s="83"/>
+      <c r="O48" s="83"/>
+      <c r="P48" s="83"/>
+      <c r="Q48" s="83"/>
+      <c r="R48" s="83"/>
+      <c r="S48" s="83"/>
+      <c r="T48" s="63"/>
+      <c r="U48" s="63"/>
+      <c r="V48" s="6"/>
     </row>
     <row r="49" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B49" s="51"/>
-      <c r="C49" s="52"/>
-      <c r="D49" s="53"/>
+      <c r="B49" s="22"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="24"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -2580,21 +3400,21 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
-      <c r="Q49" s="1"/>
-      <c r="R49" s="1"/>
-      <c r="S49" s="1"/>
-      <c r="T49" s="1"/>
-      <c r="U49" s="1"/>
-      <c r="V49" s="34"/>
+      <c r="M49" s="82"/>
+      <c r="N49" s="83"/>
+      <c r="O49" s="83"/>
+      <c r="P49" s="83"/>
+      <c r="Q49" s="83"/>
+      <c r="R49" s="83"/>
+      <c r="S49" s="83"/>
+      <c r="T49" s="63"/>
+      <c r="U49" s="63"/>
+      <c r="V49" s="6"/>
     </row>
     <row r="50" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="54"/>
-      <c r="C50" s="55"/>
-      <c r="D50" s="56"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="27"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -2603,23 +3423,23 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
-      <c r="Q50" s="1"/>
-      <c r="R50" s="1"/>
-      <c r="S50" s="1"/>
-      <c r="T50" s="1"/>
-      <c r="U50" s="1"/>
-      <c r="V50" s="34"/>
+      <c r="M50" s="82"/>
+      <c r="N50" s="83"/>
+      <c r="O50" s="83"/>
+      <c r="P50" s="83"/>
+      <c r="Q50" s="83"/>
+      <c r="R50" s="83"/>
+      <c r="S50" s="83"/>
+      <c r="T50" s="63"/>
+      <c r="U50" s="63"/>
+      <c r="V50" s="6"/>
     </row>
     <row r="51" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="57" t="s">
+      <c r="B51" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C51" s="58"/>
-      <c r="D51" s="59"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="29"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -2628,21 +3448,21 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
-      <c r="Q51" s="1"/>
-      <c r="R51" s="1"/>
-      <c r="S51" s="1"/>
-      <c r="T51" s="1"/>
-      <c r="U51" s="1"/>
-      <c r="V51" s="34"/>
+      <c r="M51" s="82"/>
+      <c r="N51" s="83"/>
+      <c r="O51" s="83"/>
+      <c r="P51" s="83"/>
+      <c r="Q51" s="83"/>
+      <c r="R51" s="83"/>
+      <c r="S51" s="83"/>
+      <c r="T51" s="63"/>
+      <c r="U51" s="63"/>
+      <c r="V51" s="6"/>
     </row>
     <row r="52" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B52" s="60"/>
-      <c r="C52" s="61"/>
-      <c r="D52" s="62"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="32"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -2651,21 +3471,21 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
-      <c r="Q52" s="1"/>
-      <c r="R52" s="1"/>
-      <c r="S52" s="1"/>
-      <c r="T52" s="1"/>
-      <c r="U52" s="1"/>
-      <c r="V52" s="34"/>
+      <c r="M52" s="82"/>
+      <c r="N52" s="83"/>
+      <c r="O52" s="83"/>
+      <c r="P52" s="83"/>
+      <c r="Q52" s="83"/>
+      <c r="R52" s="83"/>
+      <c r="S52" s="83"/>
+      <c r="T52" s="63"/>
+      <c r="U52" s="63"/>
+      <c r="V52" s="6"/>
     </row>
     <row r="53" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="63"/>
-      <c r="C53" s="64"/>
-      <c r="D53" s="65"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="35"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -2674,23 +3494,23 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
-      <c r="Q53" s="1"/>
-      <c r="R53" s="1"/>
-      <c r="S53" s="1"/>
-      <c r="T53" s="1"/>
-      <c r="U53" s="1"/>
-      <c r="V53" s="34"/>
+      <c r="M53" s="82"/>
+      <c r="N53" s="83"/>
+      <c r="O53" s="83"/>
+      <c r="P53" s="83"/>
+      <c r="Q53" s="83"/>
+      <c r="R53" s="83"/>
+      <c r="S53" s="83"/>
+      <c r="T53" s="63"/>
+      <c r="U53" s="63"/>
+      <c r="V53" s="6"/>
     </row>
     <row r="54" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="57" t="s">
+      <c r="B54" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C54" s="49"/>
-      <c r="D54" s="50"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="21"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -2699,21 +3519,21 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
-      <c r="P54" s="1"/>
-      <c r="Q54" s="1"/>
-      <c r="R54" s="1"/>
-      <c r="S54" s="1"/>
-      <c r="T54" s="1"/>
-      <c r="U54" s="1"/>
-      <c r="V54" s="34"/>
+      <c r="M54" s="82"/>
+      <c r="N54" s="83"/>
+      <c r="O54" s="83"/>
+      <c r="P54" s="83"/>
+      <c r="Q54" s="83"/>
+      <c r="R54" s="83"/>
+      <c r="S54" s="83"/>
+      <c r="T54" s="63"/>
+      <c r="U54" s="63"/>
+      <c r="V54" s="6"/>
     </row>
     <row r="55" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B55" s="51"/>
-      <c r="C55" s="52"/>
-      <c r="D55" s="53"/>
+      <c r="B55" s="22"/>
+      <c r="C55" s="23"/>
+      <c r="D55" s="24"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -2722,21 +3542,21 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
-      <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
-      <c r="O55" s="1"/>
-      <c r="P55" s="1"/>
-      <c r="Q55" s="1"/>
-      <c r="R55" s="1"/>
-      <c r="S55" s="1"/>
-      <c r="T55" s="1"/>
-      <c r="U55" s="1"/>
-      <c r="V55" s="34"/>
+      <c r="M55" s="82"/>
+      <c r="N55" s="83"/>
+      <c r="O55" s="83"/>
+      <c r="P55" s="83"/>
+      <c r="Q55" s="83"/>
+      <c r="R55" s="83"/>
+      <c r="S55" s="83"/>
+      <c r="T55" s="63"/>
+      <c r="U55" s="63"/>
+      <c r="V55" s="6"/>
     </row>
     <row r="56" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B56" s="54"/>
-      <c r="C56" s="55"/>
-      <c r="D56" s="56"/>
+      <c r="B56" s="25"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="27"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -2745,23 +3565,23 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
-      <c r="P56" s="1"/>
-      <c r="Q56" s="1"/>
-      <c r="R56" s="1"/>
-      <c r="S56" s="1"/>
-      <c r="T56" s="1"/>
-      <c r="U56" s="1"/>
-      <c r="V56" s="34"/>
+      <c r="M56" s="82"/>
+      <c r="N56" s="83"/>
+      <c r="O56" s="83"/>
+      <c r="P56" s="83"/>
+      <c r="Q56" s="83"/>
+      <c r="R56" s="83"/>
+      <c r="S56" s="83"/>
+      <c r="T56" s="63"/>
+      <c r="U56" s="63"/>
+      <c r="V56" s="6"/>
     </row>
     <row r="57" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="57" t="s">
-        <v>12</v>
-      </c>
-      <c r="C57" s="49"/>
-      <c r="D57" s="50"/>
+      <c r="B57" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="20"/>
+      <c r="D57" s="21"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -2770,21 +3590,21 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
-      <c r="M57" s="1"/>
-      <c r="N57" s="1"/>
-      <c r="O57" s="1"/>
-      <c r="P57" s="1"/>
-      <c r="Q57" s="1"/>
-      <c r="R57" s="1"/>
-      <c r="S57" s="1"/>
-      <c r="T57" s="1"/>
-      <c r="U57" s="1"/>
-      <c r="V57" s="34"/>
+      <c r="M57" s="82"/>
+      <c r="N57" s="83"/>
+      <c r="O57" s="83"/>
+      <c r="P57" s="83"/>
+      <c r="Q57" s="83"/>
+      <c r="R57" s="83"/>
+      <c r="S57" s="83"/>
+      <c r="T57" s="63"/>
+      <c r="U57" s="63"/>
+      <c r="V57" s="6"/>
     </row>
     <row r="58" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B58" s="51"/>
-      <c r="C58" s="52"/>
-      <c r="D58" s="53"/>
+      <c r="B58" s="22"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="24"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -2793,21 +3613,21 @@
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
-      <c r="O58" s="1"/>
-      <c r="P58" s="1"/>
-      <c r="Q58" s="1"/>
-      <c r="R58" s="1"/>
-      <c r="S58" s="1"/>
-      <c r="T58" s="1"/>
-      <c r="U58" s="1"/>
-      <c r="V58" s="34"/>
-    </row>
-    <row r="59" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B59" s="54"/>
-      <c r="C59" s="55"/>
-      <c r="D59" s="56"/>
+      <c r="M58" s="5"/>
+      <c r="N58" s="63"/>
+      <c r="O58" s="63"/>
+      <c r="P58" s="63"/>
+      <c r="Q58" s="63"/>
+      <c r="R58" s="63"/>
+      <c r="S58" s="63"/>
+      <c r="T58" s="63"/>
+      <c r="U58" s="63"/>
+      <c r="V58" s="6"/>
+    </row>
+    <row r="59" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B59" s="25"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="27"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -2816,23 +3636,25 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
-      <c r="N59" s="1"/>
-      <c r="O59" s="1"/>
-      <c r="P59" s="1"/>
-      <c r="Q59" s="1"/>
-      <c r="R59" s="1"/>
-      <c r="S59" s="1"/>
-      <c r="T59" s="1"/>
-      <c r="U59" s="1"/>
-      <c r="V59" s="34"/>
+      <c r="M59" s="74" t="s">
+        <v>28</v>
+      </c>
+      <c r="N59" s="67"/>
+      <c r="O59" s="67"/>
+      <c r="P59" s="85"/>
+      <c r="Q59" s="86"/>
+      <c r="R59" s="87"/>
+      <c r="S59" s="63"/>
+      <c r="T59" s="63"/>
+      <c r="U59" s="63"/>
+      <c r="V59" s="6"/>
     </row>
     <row r="60" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="57" t="s">
-        <v>8</v>
-      </c>
-      <c r="C60" s="49"/>
-      <c r="D60" s="50"/>
+      <c r="B60" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60" s="20"/>
+      <c r="D60" s="21"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -2841,21 +3663,21 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
-      <c r="M60" s="1"/>
-      <c r="N60" s="1"/>
-      <c r="O60" s="1"/>
-      <c r="P60" s="1"/>
-      <c r="Q60" s="1"/>
-      <c r="R60" s="1"/>
-      <c r="S60" s="1"/>
-      <c r="T60" s="1"/>
-      <c r="U60" s="1"/>
-      <c r="V60" s="34"/>
-    </row>
-    <row r="61" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B61" s="51"/>
-      <c r="C61" s="52"/>
-      <c r="D61" s="53"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="63"/>
+      <c r="O60" s="63"/>
+      <c r="P60" s="63"/>
+      <c r="Q60" s="63"/>
+      <c r="R60" s="63"/>
+      <c r="S60" s="63"/>
+      <c r="T60" s="63"/>
+      <c r="U60" s="63"/>
+      <c r="V60" s="6"/>
+    </row>
+    <row r="61" spans="2:22" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B61" s="22"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="24"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -2864,21 +3686,23 @@
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
-      <c r="O61" s="1"/>
-      <c r="P61" s="1"/>
-      <c r="Q61" s="1"/>
-      <c r="R61" s="1"/>
-      <c r="S61" s="1"/>
-      <c r="T61" s="1"/>
-      <c r="U61" s="1"/>
-      <c r="V61" s="34"/>
+      <c r="M61" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="N61" s="67"/>
+      <c r="O61" s="67"/>
+      <c r="P61" s="85"/>
+      <c r="Q61" s="86"/>
+      <c r="R61" s="87"/>
+      <c r="S61" s="63"/>
+      <c r="T61" s="63"/>
+      <c r="U61" s="63"/>
+      <c r="V61" s="6"/>
     </row>
     <row r="62" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B62" s="54"/>
-      <c r="C62" s="55"/>
-      <c r="D62" s="56"/>
+      <c r="B62" s="25"/>
+      <c r="C62" s="26"/>
+      <c r="D62" s="27"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -2887,23 +3711,23 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
-      <c r="M62" s="1"/>
-      <c r="N62" s="1"/>
-      <c r="O62" s="1"/>
-      <c r="P62" s="1"/>
-      <c r="Q62" s="1"/>
-      <c r="R62" s="1"/>
-      <c r="S62" s="1"/>
-      <c r="T62" s="1"/>
-      <c r="U62" s="1"/>
-      <c r="V62" s="34"/>
-    </row>
-    <row r="63" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="57" t="s">
-        <v>13</v>
-      </c>
-      <c r="C63" s="49"/>
-      <c r="D63" s="50"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="63"/>
+      <c r="O62" s="63"/>
+      <c r="P62" s="63"/>
+      <c r="Q62" s="63"/>
+      <c r="R62" s="63"/>
+      <c r="S62" s="63"/>
+      <c r="T62" s="63"/>
+      <c r="U62" s="63"/>
+      <c r="V62" s="6"/>
+    </row>
+    <row r="63" spans="2:22" ht="17" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63" s="20"/>
+      <c r="D63" s="21"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -2912,21 +3736,23 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
-      <c r="N63" s="1"/>
-      <c r="O63" s="1"/>
-      <c r="P63" s="1"/>
-      <c r="Q63" s="1"/>
-      <c r="R63" s="1"/>
-      <c r="S63" s="1"/>
-      <c r="T63" s="1"/>
-      <c r="U63" s="1"/>
-      <c r="V63" s="34"/>
+      <c r="M63" s="74" t="s">
+        <v>30</v>
+      </c>
+      <c r="N63" s="67"/>
+      <c r="O63" s="63"/>
+      <c r="P63" s="85"/>
+      <c r="Q63" s="88"/>
+      <c r="R63" s="89"/>
+      <c r="S63" s="63"/>
+      <c r="T63" s="63"/>
+      <c r="U63" s="63"/>
+      <c r="V63" s="6"/>
     </row>
     <row r="64" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B64" s="51"/>
-      <c r="C64" s="52"/>
-      <c r="D64" s="53"/>
+      <c r="B64" s="22"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="24"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -2935,22 +3761,22 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
-      <c r="M64" s="1"/>
-      <c r="N64" s="1"/>
-      <c r="O64" s="1"/>
-      <c r="P64" s="1"/>
-      <c r="Q64" s="1"/>
-      <c r="R64" s="1"/>
-      <c r="S64" s="1"/>
-      <c r="T64" s="1"/>
-      <c r="U64" s="1"/>
-      <c r="V64" s="34"/>
-    </row>
-    <row r="65" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B65" s="54"/>
-      <c r="C65" s="55"/>
-      <c r="D65" s="56"/>
-      <c r="E65" s="33"/>
+      <c r="M64" s="5"/>
+      <c r="N64" s="63"/>
+      <c r="O64" s="63"/>
+      <c r="P64" s="63"/>
+      <c r="Q64" s="63"/>
+      <c r="R64" s="63"/>
+      <c r="S64" s="63"/>
+      <c r="T64" s="63"/>
+      <c r="U64" s="63"/>
+      <c r="V64" s="6"/>
+    </row>
+    <row r="65" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B65" s="25"/>
+      <c r="C65" s="26"/>
+      <c r="D65" s="27"/>
+      <c r="E65" s="4"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
@@ -2958,24 +3784,26 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
-      <c r="M65" s="1"/>
-      <c r="N65" s="1"/>
-      <c r="O65" s="1"/>
-      <c r="P65" s="1"/>
-      <c r="Q65" s="1"/>
-      <c r="R65" s="1"/>
-      <c r="S65" s="1"/>
-      <c r="T65" s="1"/>
-      <c r="U65" s="1"/>
-      <c r="V65" s="34"/>
-    </row>
-    <row r="66" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="57" t="s">
-        <v>14</v>
-      </c>
-      <c r="C66" s="49"/>
-      <c r="D66" s="50"/>
-      <c r="E66" s="33"/>
+      <c r="M65" s="90" t="s">
+        <v>31</v>
+      </c>
+      <c r="N65" s="63"/>
+      <c r="O65" s="63"/>
+      <c r="P65" s="63"/>
+      <c r="Q65" s="63"/>
+      <c r="R65" s="63"/>
+      <c r="S65" s="63"/>
+      <c r="T65" s="63"/>
+      <c r="U65" s="63"/>
+      <c r="V65" s="6"/>
+    </row>
+    <row r="66" spans="2:22" ht="17" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" s="20"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="4"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
@@ -2983,22 +3811,24 @@
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
-      <c r="M66" s="1"/>
-      <c r="N66" s="1"/>
-      <c r="O66" s="1"/>
-      <c r="P66" s="1"/>
-      <c r="Q66" s="1"/>
-      <c r="R66" s="1"/>
-      <c r="S66" s="1"/>
-      <c r="T66" s="1"/>
-      <c r="U66" s="1"/>
-      <c r="V66" s="34"/>
+      <c r="M66" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="N66" s="67"/>
+      <c r="O66" s="63"/>
+      <c r="P66" s="63"/>
+      <c r="Q66" s="63"/>
+      <c r="R66" s="63"/>
+      <c r="S66" s="63"/>
+      <c r="T66" s="63"/>
+      <c r="U66" s="63"/>
+      <c r="V66" s="6"/>
     </row>
     <row r="67" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B67" s="51"/>
-      <c r="C67" s="52"/>
-      <c r="D67" s="53"/>
-      <c r="E67" s="33"/>
+      <c r="B67" s="22"/>
+      <c r="C67" s="23"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="4"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
@@ -3006,22 +3836,22 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
-      <c r="N67" s="1"/>
-      <c r="O67" s="1"/>
-      <c r="P67" s="1"/>
-      <c r="Q67" s="1"/>
-      <c r="R67" s="1"/>
-      <c r="S67" s="1"/>
-      <c r="T67" s="1"/>
-      <c r="U67" s="1"/>
-      <c r="V67" s="34"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="63"/>
+      <c r="O67" s="63"/>
+      <c r="P67" s="63"/>
+      <c r="Q67" s="63"/>
+      <c r="R67" s="63"/>
+      <c r="S67" s="63"/>
+      <c r="T67" s="63"/>
+      <c r="U67" s="63"/>
+      <c r="V67" s="6"/>
     </row>
     <row r="68" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B68" s="54"/>
-      <c r="C68" s="55"/>
-      <c r="D68" s="56"/>
-      <c r="E68" s="33"/>
+      <c r="B68" s="25"/>
+      <c r="C68" s="26"/>
+      <c r="D68" s="27"/>
+      <c r="E68" s="4"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
@@ -3029,24 +3859,24 @@
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
-      <c r="N68" s="1"/>
-      <c r="O68" s="1"/>
-      <c r="P68" s="1"/>
-      <c r="Q68" s="1"/>
-      <c r="R68" s="1"/>
-      <c r="S68" s="1"/>
-      <c r="T68" s="1"/>
-      <c r="U68" s="1"/>
-      <c r="V68" s="34"/>
+      <c r="M68" s="5"/>
+      <c r="N68" s="91" t="s">
+        <v>33</v>
+      </c>
+      <c r="O68" s="92"/>
+      <c r="P68" s="92"/>
+      <c r="Q68" s="92"/>
+      <c r="R68" s="92"/>
+      <c r="S68" s="92"/>
+      <c r="T68" s="92"/>
+      <c r="U68" s="93"/>
+      <c r="V68" s="6"/>
     </row>
     <row r="69" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="57" t="s">
-        <v>15</v>
-      </c>
-      <c r="C69" s="49"/>
-      <c r="D69" s="50"/>
-      <c r="E69" s="33"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="4"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
@@ -3054,22 +3884,22 @@
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
-      <c r="M69" s="1"/>
-      <c r="N69" s="1"/>
-      <c r="O69" s="1"/>
-      <c r="P69" s="1"/>
-      <c r="Q69" s="1"/>
-      <c r="R69" s="1"/>
-      <c r="S69" s="1"/>
-      <c r="T69" s="1"/>
-      <c r="U69" s="1"/>
-      <c r="V69" s="34"/>
+      <c r="M69" s="5"/>
+      <c r="N69" s="94"/>
+      <c r="O69" s="95"/>
+      <c r="P69" s="95"/>
+      <c r="Q69" s="95"/>
+      <c r="R69" s="95"/>
+      <c r="S69" s="95"/>
+      <c r="T69" s="95"/>
+      <c r="U69" s="96"/>
+      <c r="V69" s="6"/>
     </row>
     <row r="70" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B70" s="51"/>
-      <c r="C70" s="52"/>
-      <c r="D70" s="53"/>
-      <c r="E70" s="33"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="23"/>
+      <c r="D70" s="24"/>
+      <c r="E70" s="4"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
@@ -3077,55 +3907,80 @@
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
-      <c r="O70" s="1"/>
-      <c r="P70" s="1"/>
-      <c r="Q70" s="1"/>
-      <c r="R70" s="1"/>
-      <c r="S70" s="1"/>
-      <c r="T70" s="1"/>
-      <c r="U70" s="1"/>
-      <c r="V70" s="34"/>
+      <c r="M70" s="5"/>
+      <c r="N70" s="63"/>
+      <c r="O70" s="63"/>
+      <c r="P70" s="63"/>
+      <c r="Q70" s="63"/>
+      <c r="R70" s="63"/>
+      <c r="S70" s="63"/>
+      <c r="T70" s="63"/>
+      <c r="U70" s="63"/>
+      <c r="V70" s="6"/>
     </row>
     <row r="71" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B71" s="54"/>
-      <c r="C71" s="55"/>
-      <c r="D71" s="56"/>
-      <c r="E71" s="6"/>
-      <c r="F71" s="7"/>
-      <c r="G71" s="7"/>
-      <c r="H71" s="7"/>
-      <c r="I71" s="7"/>
-      <c r="J71" s="7"/>
-      <c r="K71" s="7"/>
-      <c r="L71" s="7"/>
-      <c r="M71" s="7"/>
-      <c r="N71" s="7"/>
-      <c r="O71" s="7"/>
-      <c r="P71" s="7"/>
-      <c r="Q71" s="7"/>
-      <c r="R71" s="7"/>
-      <c r="S71" s="7"/>
-      <c r="T71" s="7"/>
-      <c r="U71" s="7"/>
-      <c r="V71" s="8"/>
+      <c r="B71" s="25"/>
+      <c r="C71" s="26"/>
+      <c r="D71" s="27"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="3"/>
+      <c r="L71" s="3"/>
+      <c r="M71" s="64"/>
+      <c r="N71" s="65"/>
+      <c r="O71" s="65"/>
+      <c r="P71" s="65"/>
+      <c r="Q71" s="65"/>
+      <c r="R71" s="65"/>
+      <c r="S71" s="65"/>
+      <c r="T71" s="65"/>
+      <c r="U71" s="65"/>
+      <c r="V71" s="66"/>
     </row>
     <row r="72" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="54">
+    <mergeCell ref="M66:N66"/>
+    <mergeCell ref="N68:U69"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D13"/>
+    <mergeCell ref="B14:D15"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H12:J13"/>
+    <mergeCell ref="H14:J15"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="F41:H42"/>
+    <mergeCell ref="F43:H44"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="R34:S34"/>
+    <mergeCell ref="M59:O59"/>
+    <mergeCell ref="P59:R59"/>
+    <mergeCell ref="M61:O61"/>
+    <mergeCell ref="P61:R61"/>
+    <mergeCell ref="M63:N63"/>
+    <mergeCell ref="P63:R63"/>
     <mergeCell ref="E28:L29"/>
     <mergeCell ref="M28:V29"/>
     <mergeCell ref="B60:D62"/>
     <mergeCell ref="B63:D65"/>
     <mergeCell ref="B66:D68"/>
+    <mergeCell ref="B39:D41"/>
+    <mergeCell ref="M30:V32"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="O38:S38"/>
+    <mergeCell ref="O36:S36"/>
+    <mergeCell ref="O40:S41"/>
     <mergeCell ref="B69:D71"/>
     <mergeCell ref="F31:H36"/>
     <mergeCell ref="F37:H37"/>
     <mergeCell ref="F38:H38"/>
     <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H41"/>
-    <mergeCell ref="F42:H43"/>
     <mergeCell ref="B42:D44"/>
     <mergeCell ref="B45:D47"/>
     <mergeCell ref="B48:D50"/>
@@ -3135,19 +3990,14 @@
     <mergeCell ref="B28:D32"/>
     <mergeCell ref="B33:D35"/>
     <mergeCell ref="B36:D38"/>
-    <mergeCell ref="B39:D41"/>
+    <mergeCell ref="B2:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
     <mergeCell ref="H2:J7"/>
     <mergeCell ref="H8:J8"/>
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H11:J12"/>
-    <mergeCell ref="H13:J14"/>
-    <mergeCell ref="B2:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D12"/>
-    <mergeCell ref="B13:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Xữ lý lỗi load Framwork MetroUI, hiển thị thư viện Microsoft.Extensions.Configuration.Json và Microsoft.Extensions.Configuration Thiết kết lại layout.xlsx
</commit_message>
<xml_diff>
--- a/QuanLyCuaHangVatLieuXayDung/template/layout.xlsx
+++ b/QuanLyCuaHangVatLieuXayDung/template/layout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Phan_Tich_Va_Thiet_Ke_He_Thong_Thong_Tin\DoAnCuoiKy\QuanLyNhapXuatCuaHangVatLieuXayDung_dev_Bao\QuanLyCuaHangVatLieuXayDung\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E837C6B-5479-42EA-8D94-7909A456AEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3624D167-CEF3-419C-9172-4F8F5C425CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{30F8D3DC-B8FB-4EF1-8873-75A4B0B7C454}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>Tên: Gạch 2 lổ TCVN</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Biên lai trả nợ</t>
-  </si>
-  <si>
-    <t>Chi phí phát sinh</t>
   </si>
   <si>
     <t>Nhân viên</t>
@@ -131,9 +128,6 @@
     <t xml:space="preserve">Tiền giảm: </t>
   </si>
   <si>
-    <t>Nợ củ</t>
-  </si>
-  <si>
     <t>Tổng hóa đơn:</t>
   </si>
   <si>
@@ -148,12 +142,24 @@
   <si>
     <t>Hd00000001</t>
   </si>
+  <si>
+    <t>Kho</t>
+  </si>
+  <si>
+    <t>Thanh toán:</t>
+  </si>
+  <si>
+    <t>Nợ cũ:</t>
+  </si>
+  <si>
+    <t>Tổng nợ</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +209,28 @@
       <i/>
       <u/>
       <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -264,7 +292,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -466,55 +494,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -522,6 +506,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -642,45 +634,26 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -695,31 +668,26 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -729,6 +697,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -736,14 +707,29 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2706,8 +2692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A237127A-16A2-4193-9CBC-875260166E60}">
   <dimension ref="B1:V72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U34" sqref="U34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y51" sqref="Y51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2719,193 +2705,193 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="9"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="17"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="17"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="12"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="20"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="20"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B4" s="10"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="12"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="12"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="20"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="12"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="20"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="15"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="23"/>
     </row>
     <row r="8" spans="2:10" ht="22" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
-      <c r="H8" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="18"/>
+      <c r="B8" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="26"/>
+      <c r="H8" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="25"/>
+      <c r="J8" s="26"/>
     </row>
     <row r="9" spans="2:10" ht="22" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="18"/>
-      <c r="H9" s="16" t="s">
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
+      <c r="H9" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="I9" s="17"/>
-      <c r="J9" s="18"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="26"/>
     </row>
     <row r="10" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
-      <c r="H10" s="16" t="s">
+      <c r="C10" s="25"/>
+      <c r="D10" s="26"/>
+      <c r="H10" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="17"/>
-      <c r="J10" s="18"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="26"/>
     </row>
     <row r="11" spans="2:10" ht="16" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
-      <c r="H11" s="16" t="s">
+      <c r="C11" s="25"/>
+      <c r="D11" s="26"/>
+      <c r="H11" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="I11" s="17"/>
-      <c r="J11" s="18"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="26"/>
     </row>
     <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="105" t="s">
+      <c r="B12" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="97"/>
-      <c r="D12" s="98"/>
-      <c r="H12" s="105" t="s">
+      <c r="C12" s="91"/>
+      <c r="D12" s="92"/>
+      <c r="H12" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="I12" s="97"/>
-      <c r="J12" s="98"/>
+      <c r="I12" s="91"/>
+      <c r="J12" s="92"/>
     </row>
     <row r="13" spans="2:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="99"/>
-      <c r="C13" s="97"/>
-      <c r="D13" s="98"/>
-      <c r="H13" s="99"/>
-      <c r="I13" s="97"/>
-      <c r="J13" s="98"/>
+      <c r="B13" s="93"/>
+      <c r="C13" s="91"/>
+      <c r="D13" s="92"/>
+      <c r="H13" s="93"/>
+      <c r="I13" s="91"/>
+      <c r="J13" s="92"/>
     </row>
     <row r="14" spans="2:10" ht="13" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="106" t="s">
+      <c r="B14" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="100"/>
-      <c r="D14" s="101"/>
-      <c r="H14" s="106" t="s">
+      <c r="C14" s="95"/>
+      <c r="D14" s="96"/>
+      <c r="H14" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="I14" s="100"/>
-      <c r="J14" s="101"/>
+      <c r="I14" s="95"/>
+      <c r="J14" s="96"/>
     </row>
     <row r="15" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="102"/>
-      <c r="C15" s="103"/>
-      <c r="D15" s="104"/>
-      <c r="H15" s="102"/>
-      <c r="I15" s="103"/>
-      <c r="J15" s="104"/>
+      <c r="B15" s="97"/>
+      <c r="C15" s="98"/>
+      <c r="D15" s="99"/>
+      <c r="H15" s="97"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="99"/>
     </row>
     <row r="16" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="28" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="36"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="58"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="58"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="58"/>
-      <c r="K28" s="58"/>
-      <c r="L28" s="58"/>
-      <c r="M28" s="61"/>
-      <c r="N28" s="61"/>
-      <c r="O28" s="61"/>
-      <c r="P28" s="61"/>
-      <c r="Q28" s="61"/>
-      <c r="R28" s="61"/>
-      <c r="S28" s="61"/>
-      <c r="T28" s="61"/>
-      <c r="U28" s="61"/>
-      <c r="V28" s="62"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="84"/>
+      <c r="F28" s="85"/>
+      <c r="G28" s="85"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="85"/>
+      <c r="J28" s="85"/>
+      <c r="K28" s="85"/>
+      <c r="L28" s="85"/>
+      <c r="M28" s="88"/>
+      <c r="N28" s="88"/>
+      <c r="O28" s="88"/>
+      <c r="P28" s="88"/>
+      <c r="Q28" s="88"/>
+      <c r="R28" s="88"/>
+      <c r="S28" s="88"/>
+      <c r="T28" s="88"/>
+      <c r="U28" s="88"/>
+      <c r="V28" s="89"/>
     </row>
     <row r="29" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="39"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="60"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="60"/>
-      <c r="J29" s="60"/>
-      <c r="K29" s="60"/>
-      <c r="L29" s="60"/>
-      <c r="M29" s="46"/>
-      <c r="N29" s="46"/>
-      <c r="O29" s="46"/>
-      <c r="P29" s="46"/>
-      <c r="Q29" s="46"/>
-      <c r="R29" s="46"/>
-      <c r="S29" s="46"/>
-      <c r="T29" s="46"/>
-      <c r="U29" s="46"/>
-      <c r="V29" s="47"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
+      <c r="H29" s="87"/>
+      <c r="I29" s="87"/>
+      <c r="J29" s="87"/>
+      <c r="K29" s="87"/>
+      <c r="L29" s="87"/>
+      <c r="M29" s="54"/>
+      <c r="N29" s="54"/>
+      <c r="O29" s="54"/>
+      <c r="P29" s="54"/>
+      <c r="Q29" s="54"/>
+      <c r="R29" s="54"/>
+      <c r="S29" s="54"/>
+      <c r="T29" s="54"/>
+      <c r="U29" s="54"/>
+      <c r="V29" s="55"/>
     </row>
     <row r="30" spans="2:22" ht="6.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="39"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="41"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="49"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -2914,413 +2900,413 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
-      <c r="M30" s="68" t="s">
-        <v>16</v>
-      </c>
-      <c r="N30" s="69"/>
-      <c r="O30" s="69"/>
-      <c r="P30" s="69"/>
-      <c r="Q30" s="69"/>
-      <c r="R30" s="69"/>
-      <c r="S30" s="69"/>
-      <c r="T30" s="69"/>
-      <c r="U30" s="69"/>
-      <c r="V30" s="70"/>
+      <c r="M30" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="N30" s="66"/>
+      <c r="O30" s="66"/>
+      <c r="P30" s="66"/>
+      <c r="Q30" s="66"/>
+      <c r="R30" s="66"/>
+      <c r="S30" s="66"/>
+      <c r="T30" s="66"/>
+      <c r="U30" s="66"/>
+      <c r="V30" s="67"/>
     </row>
     <row r="31" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="42"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="44"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="52"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="9"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="17"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
-      <c r="M31" s="71"/>
-      <c r="N31" s="72"/>
-      <c r="O31" s="72"/>
-      <c r="P31" s="72"/>
-      <c r="Q31" s="72"/>
-      <c r="R31" s="72"/>
-      <c r="S31" s="72"/>
-      <c r="T31" s="72"/>
-      <c r="U31" s="72"/>
-      <c r="V31" s="73"/>
+      <c r="M31" s="68"/>
+      <c r="N31" s="69"/>
+      <c r="O31" s="69"/>
+      <c r="P31" s="69"/>
+      <c r="Q31" s="69"/>
+      <c r="R31" s="69"/>
+      <c r="S31" s="69"/>
+      <c r="T31" s="69"/>
+      <c r="U31" s="69"/>
+      <c r="V31" s="70"/>
     </row>
     <row r="32" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="45"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="47"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="55"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="12"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="20"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
-      <c r="M32" s="71"/>
-      <c r="N32" s="72"/>
-      <c r="O32" s="72"/>
-      <c r="P32" s="72"/>
-      <c r="Q32" s="72"/>
-      <c r="R32" s="72"/>
-      <c r="S32" s="72"/>
-      <c r="T32" s="72"/>
-      <c r="U32" s="72"/>
-      <c r="V32" s="73"/>
+      <c r="M32" s="68"/>
+      <c r="N32" s="69"/>
+      <c r="O32" s="69"/>
+      <c r="P32" s="69"/>
+      <c r="Q32" s="69"/>
+      <c r="R32" s="69"/>
+      <c r="S32" s="69"/>
+      <c r="T32" s="69"/>
+      <c r="U32" s="69"/>
+      <c r="V32" s="70"/>
     </row>
     <row r="33" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="48" t="s">
+      <c r="B33" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="49"/>
-      <c r="D33" s="50"/>
+      <c r="C33" s="57"/>
+      <c r="D33" s="58"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="12"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="20"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="5"/>
-      <c r="N33" s="63"/>
-      <c r="O33" s="63"/>
-      <c r="P33" s="63"/>
-      <c r="Q33" s="63"/>
-      <c r="R33" s="63"/>
-      <c r="S33" s="63"/>
-      <c r="T33" s="63"/>
-      <c r="U33" s="63"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
       <c r="V33" s="6"/>
     </row>
     <row r="34" spans="2:22" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B34" s="51"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="53"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="61"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="12"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="20"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
-      <c r="M34" s="74" t="s">
-        <v>35</v>
-      </c>
-      <c r="N34" s="67"/>
-      <c r="O34" s="108" t="s">
-        <v>36</v>
-      </c>
-      <c r="P34" s="89"/>
-      <c r="Q34" s="107"/>
-      <c r="R34" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="S34" s="67"/>
-      <c r="T34" s="107"/>
-      <c r="U34" s="63"/>
+      <c r="M34" s="71" t="s">
+        <v>33</v>
+      </c>
+      <c r="N34" s="72"/>
+      <c r="O34" s="100" t="s">
+        <v>34</v>
+      </c>
+      <c r="P34" s="83"/>
+      <c r="Q34" s="14"/>
+      <c r="R34" s="101" t="s">
+        <v>16</v>
+      </c>
+      <c r="S34" s="72"/>
+      <c r="T34" s="14"/>
+      <c r="U34" s="7"/>
       <c r="V34" s="6"/>
     </row>
     <row r="35" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="54"/>
-      <c r="C35" s="55"/>
-      <c r="D35" s="56"/>
+      <c r="B35" s="62"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="64"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="12"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="20"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="5"/>
-      <c r="N35" s="63"/>
-      <c r="O35" s="63"/>
-      <c r="P35" s="63"/>
-      <c r="Q35" s="63"/>
-      <c r="R35" s="63"/>
-      <c r="S35" s="63"/>
-      <c r="T35" s="63"/>
-      <c r="U35" s="63"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
       <c r="V35" s="6"/>
     </row>
     <row r="36" spans="2:22" ht="17" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="21"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="29"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="15"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="23"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
-      <c r="M36" s="76" t="s">
-        <v>18</v>
-      </c>
-      <c r="N36" s="77"/>
-      <c r="O36" s="80"/>
-      <c r="P36" s="67"/>
-      <c r="Q36" s="67"/>
-      <c r="R36" s="67"/>
-      <c r="S36" s="67"/>
-      <c r="T36" s="63"/>
-      <c r="U36" s="63"/>
+      <c r="M36" s="73" t="s">
+        <v>17</v>
+      </c>
+      <c r="N36" s="74"/>
+      <c r="O36" s="77"/>
+      <c r="P36" s="72"/>
+      <c r="Q36" s="72"/>
+      <c r="R36" s="72"/>
+      <c r="S36" s="72"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
       <c r="V36" s="6"/>
     </row>
     <row r="37" spans="2:22" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B37" s="22"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="24"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="32"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="G37" s="17"/>
-      <c r="H37" s="18"/>
+      <c r="F37" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="G37" s="25"/>
+      <c r="H37" s="26"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="5"/>
-      <c r="N37" s="63"/>
-      <c r="O37" s="63"/>
-      <c r="P37" s="63"/>
-      <c r="Q37" s="63"/>
-      <c r="R37" s="63"/>
-      <c r="S37" s="63"/>
-      <c r="T37" s="63"/>
-      <c r="U37" s="63"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="7"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
+      <c r="U37" s="7"/>
       <c r="V37" s="6"/>
     </row>
     <row r="38" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="25"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="27"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="35"/>
       <c r="E38" s="1"/>
-      <c r="F38" s="16" t="s">
+      <c r="F38" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="G38" s="17"/>
-      <c r="H38" s="18"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="26"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
-      <c r="M38" s="78" t="s">
-        <v>19</v>
-      </c>
-      <c r="N38" s="79"/>
-      <c r="O38" s="80"/>
-      <c r="P38" s="81"/>
-      <c r="Q38" s="81"/>
-      <c r="R38" s="81"/>
-      <c r="S38" s="81"/>
-      <c r="T38" s="63"/>
-      <c r="U38" s="63"/>
+      <c r="M38" s="75" t="s">
+        <v>18</v>
+      </c>
+      <c r="N38" s="76"/>
+      <c r="O38" s="77"/>
+      <c r="P38" s="78"/>
+      <c r="Q38" s="78"/>
+      <c r="R38" s="78"/>
+      <c r="S38" s="78"/>
+      <c r="T38" s="7"/>
+      <c r="U38" s="7"/>
       <c r="V38" s="6"/>
     </row>
     <row r="39" spans="2:22" ht="17" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="20"/>
-      <c r="D39" s="21"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="29"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="16" t="s">
+      <c r="F39" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="G39" s="17"/>
-      <c r="H39" s="18"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="26"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="5"/>
-      <c r="N39" s="63"/>
-      <c r="O39" s="63"/>
-      <c r="P39" s="63"/>
-      <c r="Q39" s="63"/>
-      <c r="R39" s="63"/>
-      <c r="S39" s="63"/>
-      <c r="T39" s="63"/>
-      <c r="U39" s="63"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
+      <c r="U39" s="7"/>
       <c r="V39" s="6"/>
     </row>
     <row r="40" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="22"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="24"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="32"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="16" t="s">
+      <c r="F40" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="G40" s="17"/>
-      <c r="H40" s="18"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="26"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="N40" s="63"/>
-      <c r="O40" s="80"/>
-      <c r="P40" s="81"/>
-      <c r="Q40" s="81"/>
-      <c r="R40" s="81"/>
-      <c r="S40" s="81"/>
-      <c r="T40" s="63"/>
-      <c r="U40" s="63"/>
+        <v>19</v>
+      </c>
+      <c r="N40" s="7"/>
+      <c r="O40" s="77"/>
+      <c r="P40" s="78"/>
+      <c r="Q40" s="78"/>
+      <c r="R40" s="78"/>
+      <c r="S40" s="78"/>
+      <c r="T40" s="7"/>
+      <c r="U40" s="7"/>
       <c r="V40" s="6"/>
     </row>
     <row r="41" spans="2:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="25"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="27"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="35"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="105" t="s">
+      <c r="F41" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="G41" s="97"/>
-      <c r="H41" s="98"/>
+      <c r="G41" s="91"/>
+      <c r="H41" s="92"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="5"/>
-      <c r="N41" s="63"/>
-      <c r="O41" s="81"/>
-      <c r="P41" s="81"/>
-      <c r="Q41" s="81"/>
-      <c r="R41" s="81"/>
-      <c r="S41" s="81"/>
-      <c r="T41" s="63"/>
-      <c r="U41" s="63"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="78"/>
+      <c r="P41" s="78"/>
+      <c r="Q41" s="78"/>
+      <c r="R41" s="78"/>
+      <c r="S41" s="78"/>
+      <c r="T41" s="7"/>
+      <c r="U41" s="7"/>
       <c r="V41" s="6"/>
     </row>
     <row r="42" spans="2:22" ht="15.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C42" s="28"/>
-      <c r="D42" s="29"/>
+      <c r="B42" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" s="36"/>
+      <c r="D42" s="37"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="99"/>
-      <c r="G42" s="97"/>
-      <c r="H42" s="98"/>
+      <c r="F42" s="93"/>
+      <c r="G42" s="91"/>
+      <c r="H42" s="92"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="5"/>
-      <c r="N42" s="63"/>
-      <c r="O42" s="63"/>
-      <c r="P42" s="63"/>
-      <c r="Q42" s="63"/>
-      <c r="R42" s="63"/>
-      <c r="S42" s="63"/>
-      <c r="T42" s="63"/>
-      <c r="U42" s="63"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
+      <c r="S42" s="7"/>
+      <c r="T42" s="7"/>
+      <c r="U42" s="7"/>
       <c r="V42" s="6"/>
     </row>
     <row r="43" spans="2:22" ht="15.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="30"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="32"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="40"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="106" t="s">
+      <c r="F43" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="G43" s="100"/>
-      <c r="H43" s="101"/>
+      <c r="G43" s="95"/>
+      <c r="H43" s="96"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
-      <c r="M43" s="84" t="s">
+      <c r="M43" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="N43" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="N43" s="84" t="s">
+      <c r="O43" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="O43" s="84" t="s">
+      <c r="P43" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="P43" s="84" t="s">
+      <c r="Q43" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="Q43" s="84" t="s">
+      <c r="R43" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="R43" s="84" t="s">
+      <c r="S43" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="S43" s="84" t="s">
-        <v>27</v>
-      </c>
-      <c r="T43" s="63"/>
-      <c r="U43" s="63"/>
+      <c r="T43" s="7"/>
+      <c r="U43" s="7"/>
       <c r="V43" s="6"/>
     </row>
     <row r="44" spans="2:22" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="33"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="35"/>
+      <c r="B44" s="41"/>
+      <c r="C44" s="42"/>
+      <c r="D44" s="43"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="102"/>
-      <c r="G44" s="103"/>
-      <c r="H44" s="104"/>
+      <c r="F44" s="97"/>
+      <c r="G44" s="98"/>
+      <c r="H44" s="99"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
-      <c r="M44" s="82"/>
-      <c r="N44" s="83"/>
-      <c r="O44" s="83"/>
-      <c r="P44" s="83"/>
-      <c r="Q44" s="83"/>
-      <c r="R44" s="83"/>
-      <c r="S44" s="83"/>
-      <c r="T44" s="63"/>
-      <c r="U44" s="63"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="12"/>
+      <c r="O44" s="12"/>
+      <c r="P44" s="12"/>
+      <c r="Q44" s="12"/>
+      <c r="R44" s="12"/>
+      <c r="S44" s="12"/>
+      <c r="T44" s="7"/>
+      <c r="U44" s="7"/>
       <c r="V44" s="6"/>
     </row>
     <row r="45" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" s="20"/>
-      <c r="D45" s="21"/>
+      <c r="B45" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="28"/>
+      <c r="D45" s="29"/>
       <c r="E45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
-      <c r="M45" s="82"/>
-      <c r="N45" s="83"/>
-      <c r="O45" s="83"/>
-      <c r="P45" s="83"/>
-      <c r="Q45" s="83"/>
-      <c r="R45" s="83"/>
-      <c r="S45" s="83"/>
-      <c r="T45" s="63"/>
-      <c r="U45" s="63"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="12"/>
+      <c r="O45" s="12"/>
+      <c r="P45" s="12"/>
+      <c r="Q45" s="12"/>
+      <c r="R45" s="12"/>
+      <c r="S45" s="12"/>
+      <c r="T45" s="7"/>
+      <c r="U45" s="7"/>
       <c r="V45" s="6"/>
     </row>
     <row r="46" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B46" s="22"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="24"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="32"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -3329,21 +3315,21 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
-      <c r="M46" s="82"/>
-      <c r="N46" s="83"/>
-      <c r="O46" s="83"/>
-      <c r="P46" s="83"/>
-      <c r="Q46" s="83"/>
-      <c r="R46" s="83"/>
-      <c r="S46" s="83"/>
-      <c r="T46" s="63"/>
-      <c r="U46" s="63"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="12"/>
+      <c r="O46" s="12"/>
+      <c r="P46" s="12"/>
+      <c r="Q46" s="12"/>
+      <c r="R46" s="12"/>
+      <c r="S46" s="12"/>
+      <c r="T46" s="7"/>
+      <c r="U46" s="7"/>
       <c r="V46" s="6"/>
     </row>
     <row r="47" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="25"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="27"/>
+      <c r="B47" s="33"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="35"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -3352,23 +3338,23 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
-      <c r="M47" s="82"/>
-      <c r="N47" s="83"/>
-      <c r="O47" s="83"/>
-      <c r="P47" s="83"/>
-      <c r="Q47" s="83"/>
-      <c r="R47" s="83"/>
-      <c r="S47" s="83"/>
-      <c r="T47" s="63"/>
-      <c r="U47" s="63"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="12"/>
+      <c r="O47" s="12"/>
+      <c r="P47" s="12"/>
+      <c r="Q47" s="12"/>
+      <c r="R47" s="12"/>
+      <c r="S47" s="12"/>
+      <c r="T47" s="7"/>
+      <c r="U47" s="7"/>
       <c r="V47" s="6"/>
     </row>
     <row r="48" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" s="20"/>
-      <c r="D48" s="21"/>
+      <c r="B48" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="28"/>
+      <c r="D48" s="29"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -3377,21 +3363,21 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
-      <c r="M48" s="82"/>
-      <c r="N48" s="83"/>
-      <c r="O48" s="83"/>
-      <c r="P48" s="83"/>
-      <c r="Q48" s="83"/>
-      <c r="R48" s="83"/>
-      <c r="S48" s="83"/>
-      <c r="T48" s="63"/>
-      <c r="U48" s="63"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="12"/>
+      <c r="O48" s="12"/>
+      <c r="P48" s="12"/>
+      <c r="Q48" s="12"/>
+      <c r="R48" s="12"/>
+      <c r="S48" s="12"/>
+      <c r="T48" s="7"/>
+      <c r="U48" s="7"/>
       <c r="V48" s="6"/>
     </row>
     <row r="49" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B49" s="22"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="24"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="32"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -3400,21 +3386,21 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
-      <c r="M49" s="82"/>
-      <c r="N49" s="83"/>
-      <c r="O49" s="83"/>
-      <c r="P49" s="83"/>
-      <c r="Q49" s="83"/>
-      <c r="R49" s="83"/>
-      <c r="S49" s="83"/>
-      <c r="T49" s="63"/>
-      <c r="U49" s="63"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="12"/>
+      <c r="O49" s="12"/>
+      <c r="P49" s="12"/>
+      <c r="Q49" s="12"/>
+      <c r="R49" s="12"/>
+      <c r="S49" s="12"/>
+      <c r="T49" s="7"/>
+      <c r="U49" s="7"/>
       <c r="V49" s="6"/>
     </row>
     <row r="50" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="25"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="27"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="35"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -3423,23 +3409,23 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
-      <c r="M50" s="82"/>
-      <c r="N50" s="83"/>
-      <c r="O50" s="83"/>
-      <c r="P50" s="83"/>
-      <c r="Q50" s="83"/>
-      <c r="R50" s="83"/>
-      <c r="S50" s="83"/>
-      <c r="T50" s="63"/>
-      <c r="U50" s="63"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="12"/>
+      <c r="O50" s="12"/>
+      <c r="P50" s="12"/>
+      <c r="Q50" s="12"/>
+      <c r="R50" s="12"/>
+      <c r="S50" s="12"/>
+      <c r="T50" s="7"/>
+      <c r="U50" s="7"/>
       <c r="V50" s="6"/>
     </row>
     <row r="51" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C51" s="28"/>
-      <c r="D51" s="29"/>
+      <c r="B51" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="36"/>
+      <c r="D51" s="37"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -3448,21 +3434,21 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
-      <c r="M51" s="82"/>
-      <c r="N51" s="83"/>
-      <c r="O51" s="83"/>
-      <c r="P51" s="83"/>
-      <c r="Q51" s="83"/>
-      <c r="R51" s="83"/>
-      <c r="S51" s="83"/>
-      <c r="T51" s="63"/>
-      <c r="U51" s="63"/>
+      <c r="M51" s="11"/>
+      <c r="N51" s="12"/>
+      <c r="O51" s="12"/>
+      <c r="P51" s="12"/>
+      <c r="Q51" s="12"/>
+      <c r="R51" s="12"/>
+      <c r="S51" s="12"/>
+      <c r="T51" s="7"/>
+      <c r="U51" s="7"/>
       <c r="V51" s="6"/>
     </row>
     <row r="52" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B52" s="30"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="32"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="39"/>
+      <c r="D52" s="40"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -3471,21 +3457,21 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
-      <c r="M52" s="82"/>
-      <c r="N52" s="83"/>
-      <c r="O52" s="83"/>
-      <c r="P52" s="83"/>
-      <c r="Q52" s="83"/>
-      <c r="R52" s="83"/>
-      <c r="S52" s="83"/>
-      <c r="T52" s="63"/>
-      <c r="U52" s="63"/>
+      <c r="M52" s="11"/>
+      <c r="N52" s="12"/>
+      <c r="O52" s="12"/>
+      <c r="P52" s="12"/>
+      <c r="Q52" s="12"/>
+      <c r="R52" s="12"/>
+      <c r="S52" s="12"/>
+      <c r="T52" s="7"/>
+      <c r="U52" s="7"/>
       <c r="V52" s="6"/>
     </row>
     <row r="53" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="33"/>
-      <c r="C53" s="34"/>
-      <c r="D53" s="35"/>
+      <c r="B53" s="41"/>
+      <c r="C53" s="42"/>
+      <c r="D53" s="43"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -3494,23 +3480,23 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
-      <c r="M53" s="82"/>
-      <c r="N53" s="83"/>
-      <c r="O53" s="83"/>
-      <c r="P53" s="83"/>
-      <c r="Q53" s="83"/>
-      <c r="R53" s="83"/>
-      <c r="S53" s="83"/>
-      <c r="T53" s="63"/>
-      <c r="U53" s="63"/>
+      <c r="M53" s="11"/>
+      <c r="N53" s="12"/>
+      <c r="O53" s="12"/>
+      <c r="P53" s="12"/>
+      <c r="Q53" s="12"/>
+      <c r="R53" s="12"/>
+      <c r="S53" s="12"/>
+      <c r="T53" s="7"/>
+      <c r="U53" s="7"/>
       <c r="V53" s="6"/>
     </row>
     <row r="54" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C54" s="20"/>
-      <c r="D54" s="21"/>
+      <c r="B54" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" s="28"/>
+      <c r="D54" s="29"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -3519,21 +3505,21 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
-      <c r="M54" s="82"/>
-      <c r="N54" s="83"/>
-      <c r="O54" s="83"/>
-      <c r="P54" s="83"/>
-      <c r="Q54" s="83"/>
-      <c r="R54" s="83"/>
-      <c r="S54" s="83"/>
-      <c r="T54" s="63"/>
-      <c r="U54" s="63"/>
+      <c r="M54" s="11"/>
+      <c r="N54" s="12"/>
+      <c r="O54" s="12"/>
+      <c r="P54" s="12"/>
+      <c r="Q54" s="12"/>
+      <c r="R54" s="12"/>
+      <c r="S54" s="12"/>
+      <c r="T54" s="7"/>
+      <c r="U54" s="7"/>
       <c r="V54" s="6"/>
     </row>
     <row r="55" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B55" s="22"/>
-      <c r="C55" s="23"/>
-      <c r="D55" s="24"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="32"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -3542,21 +3528,21 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
-      <c r="M55" s="82"/>
-      <c r="N55" s="83"/>
-      <c r="O55" s="83"/>
-      <c r="P55" s="83"/>
-      <c r="Q55" s="83"/>
-      <c r="R55" s="83"/>
-      <c r="S55" s="83"/>
-      <c r="T55" s="63"/>
-      <c r="U55" s="63"/>
+      <c r="M55" s="11"/>
+      <c r="N55" s="12"/>
+      <c r="O55" s="12"/>
+      <c r="P55" s="12"/>
+      <c r="Q55" s="12"/>
+      <c r="R55" s="12"/>
+      <c r="S55" s="12"/>
+      <c r="T55" s="7"/>
+      <c r="U55" s="7"/>
       <c r="V55" s="6"/>
     </row>
     <row r="56" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B56" s="25"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="27"/>
+      <c r="B56" s="33"/>
+      <c r="C56" s="34"/>
+      <c r="D56" s="35"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -3565,23 +3551,23 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
-      <c r="M56" s="82"/>
-      <c r="N56" s="83"/>
-      <c r="O56" s="83"/>
-      <c r="P56" s="83"/>
-      <c r="Q56" s="83"/>
-      <c r="R56" s="83"/>
-      <c r="S56" s="83"/>
-      <c r="T56" s="63"/>
-      <c r="U56" s="63"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="12"/>
+      <c r="O56" s="12"/>
+      <c r="P56" s="12"/>
+      <c r="Q56" s="12"/>
+      <c r="R56" s="12"/>
+      <c r="S56" s="12"/>
+      <c r="T56" s="7"/>
+      <c r="U56" s="7"/>
       <c r="V56" s="6"/>
     </row>
     <row r="57" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="19" t="s">
+      <c r="B57" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="20"/>
-      <c r="D57" s="21"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="29"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -3590,21 +3576,21 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
-      <c r="M57" s="82"/>
-      <c r="N57" s="83"/>
-      <c r="O57" s="83"/>
-      <c r="P57" s="83"/>
-      <c r="Q57" s="83"/>
-      <c r="R57" s="83"/>
-      <c r="S57" s="83"/>
-      <c r="T57" s="63"/>
-      <c r="U57" s="63"/>
+      <c r="M57" s="11"/>
+      <c r="N57" s="12"/>
+      <c r="O57" s="12"/>
+      <c r="P57" s="12"/>
+      <c r="Q57" s="12"/>
+      <c r="R57" s="12"/>
+      <c r="S57" s="12"/>
+      <c r="T57" s="7"/>
+      <c r="U57" s="7"/>
       <c r="V57" s="6"/>
     </row>
     <row r="58" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B58" s="22"/>
-      <c r="C58" s="23"/>
-      <c r="D58" s="24"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="31"/>
+      <c r="D58" s="32"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -3614,20 +3600,20 @@
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
       <c r="M58" s="5"/>
-      <c r="N58" s="63"/>
-      <c r="O58" s="63"/>
-      <c r="P58" s="63"/>
-      <c r="Q58" s="63"/>
-      <c r="R58" s="63"/>
-      <c r="S58" s="63"/>
-      <c r="T58" s="63"/>
-      <c r="U58" s="63"/>
+      <c r="N58" s="7"/>
+      <c r="O58" s="7"/>
+      <c r="P58" s="7"/>
+      <c r="Q58" s="7"/>
+      <c r="R58" s="7"/>
+      <c r="S58" s="7"/>
+      <c r="T58" s="7"/>
+      <c r="U58" s="7"/>
       <c r="V58" s="6"/>
     </row>
     <row r="59" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B59" s="25"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="27"/>
+      <c r="B59" s="33"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="35"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -3636,25 +3622,25 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
-      <c r="M59" s="74" t="s">
-        <v>28</v>
-      </c>
-      <c r="N59" s="67"/>
-      <c r="O59" s="67"/>
-      <c r="P59" s="85"/>
-      <c r="Q59" s="86"/>
-      <c r="R59" s="87"/>
-      <c r="S59" s="63"/>
-      <c r="T59" s="63"/>
-      <c r="U59" s="63"/>
+      <c r="M59" s="71" t="s">
+        <v>27</v>
+      </c>
+      <c r="N59" s="72"/>
+      <c r="O59" s="72"/>
+      <c r="P59" s="79"/>
+      <c r="Q59" s="80"/>
+      <c r="R59" s="81"/>
+      <c r="S59" s="7"/>
+      <c r="T59" s="7"/>
+      <c r="U59" s="7"/>
       <c r="V59" s="6"/>
     </row>
     <row r="60" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C60" s="20"/>
-      <c r="D60" s="21"/>
+      <c r="B60" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C60" s="28"/>
+      <c r="D60" s="29"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -3664,20 +3650,20 @@
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
       <c r="M60" s="5"/>
-      <c r="N60" s="63"/>
-      <c r="O60" s="63"/>
-      <c r="P60" s="63"/>
-      <c r="Q60" s="63"/>
-      <c r="R60" s="63"/>
-      <c r="S60" s="63"/>
-      <c r="T60" s="63"/>
-      <c r="U60" s="63"/>
+      <c r="N60" s="7"/>
+      <c r="O60" s="7"/>
+      <c r="P60" s="7"/>
+      <c r="Q60" s="7"/>
+      <c r="R60" s="7"/>
+      <c r="S60" s="7"/>
+      <c r="T60" s="7"/>
+      <c r="U60" s="7"/>
       <c r="V60" s="6"/>
     </row>
     <row r="61" spans="2:22" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="B61" s="22"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="24"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="32"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -3686,23 +3672,23 @@
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
-      <c r="M61" s="74" t="s">
-        <v>29</v>
-      </c>
-      <c r="N61" s="67"/>
-      <c r="O61" s="67"/>
-      <c r="P61" s="85"/>
-      <c r="Q61" s="86"/>
-      <c r="R61" s="87"/>
-      <c r="S61" s="63"/>
-      <c r="T61" s="63"/>
-      <c r="U61" s="63"/>
+      <c r="M61" s="71" t="s">
+        <v>28</v>
+      </c>
+      <c r="N61" s="72"/>
+      <c r="O61" s="72"/>
+      <c r="P61" s="79"/>
+      <c r="Q61" s="80"/>
+      <c r="R61" s="81"/>
+      <c r="S61" s="7"/>
+      <c r="T61" s="7"/>
+      <c r="U61" s="7"/>
       <c r="V61" s="6"/>
     </row>
     <row r="62" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B62" s="25"/>
-      <c r="C62" s="26"/>
-      <c r="D62" s="27"/>
+      <c r="B62" s="33"/>
+      <c r="C62" s="34"/>
+      <c r="D62" s="35"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -3712,22 +3698,22 @@
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="5"/>
-      <c r="N62" s="63"/>
-      <c r="O62" s="63"/>
-      <c r="P62" s="63"/>
-      <c r="Q62" s="63"/>
-      <c r="R62" s="63"/>
-      <c r="S62" s="63"/>
-      <c r="T62" s="63"/>
-      <c r="U62" s="63"/>
+      <c r="N62" s="7"/>
+      <c r="O62" s="7"/>
+      <c r="P62" s="7"/>
+      <c r="Q62" s="7"/>
+      <c r="R62" s="7"/>
+      <c r="S62" s="7"/>
+      <c r="T62" s="7"/>
+      <c r="U62" s="7"/>
       <c r="V62" s="6"/>
     </row>
     <row r="63" spans="2:22" ht="17" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C63" s="20"/>
-      <c r="D63" s="21"/>
+      <c r="B63" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="28"/>
+      <c r="D63" s="29"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -3736,23 +3722,23 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
-      <c r="M63" s="74" t="s">
-        <v>30</v>
-      </c>
-      <c r="N63" s="67"/>
-      <c r="O63" s="63"/>
-      <c r="P63" s="85"/>
-      <c r="Q63" s="88"/>
-      <c r="R63" s="89"/>
-      <c r="S63" s="63"/>
-      <c r="T63" s="63"/>
-      <c r="U63" s="63"/>
+      <c r="M63" s="71" t="s">
+        <v>29</v>
+      </c>
+      <c r="N63" s="72"/>
+      <c r="O63" s="7"/>
+      <c r="P63" s="79"/>
+      <c r="Q63" s="82"/>
+      <c r="R63" s="83"/>
+      <c r="S63" s="7"/>
+      <c r="T63" s="7"/>
+      <c r="U63" s="7"/>
       <c r="V63" s="6"/>
     </row>
-    <row r="64" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B64" s="22"/>
-      <c r="C64" s="23"/>
-      <c r="D64" s="24"/>
+    <row r="64" spans="2:22" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="B64" s="30"/>
+      <c r="C64" s="31"/>
+      <c r="D64" s="32"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -3761,21 +3747,23 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
-      <c r="M64" s="5"/>
-      <c r="N64" s="63"/>
-      <c r="O64" s="63"/>
-      <c r="P64" s="63"/>
-      <c r="Q64" s="63"/>
-      <c r="R64" s="63"/>
-      <c r="S64" s="63"/>
-      <c r="T64" s="63"/>
-      <c r="U64" s="63"/>
+      <c r="M64" s="71" t="s">
+        <v>30</v>
+      </c>
+      <c r="N64" s="72"/>
+      <c r="O64" s="7"/>
+      <c r="P64" s="7"/>
+      <c r="Q64" s="7"/>
+      <c r="R64" s="7"/>
+      <c r="S64" s="7"/>
+      <c r="T64" s="7"/>
+      <c r="U64" s="7"/>
       <c r="V64" s="6"/>
     </row>
     <row r="65" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B65" s="25"/>
-      <c r="C65" s="26"/>
-      <c r="D65" s="27"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="34"/>
+      <c r="D65" s="35"/>
       <c r="E65" s="4"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
@@ -3784,25 +3772,25 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
-      <c r="M65" s="90" t="s">
-        <v>31</v>
-      </c>
-      <c r="N65" s="63"/>
-      <c r="O65" s="63"/>
-      <c r="P65" s="63"/>
-      <c r="Q65" s="63"/>
-      <c r="R65" s="63"/>
-      <c r="S65" s="63"/>
-      <c r="T65" s="63"/>
-      <c r="U65" s="63"/>
+      <c r="M65" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="N65" s="72"/>
+      <c r="O65" s="7"/>
+      <c r="P65" s="7"/>
+      <c r="Q65" s="7"/>
+      <c r="R65" s="7"/>
+      <c r="S65" s="7"/>
+      <c r="T65" s="7"/>
+      <c r="U65" s="7"/>
       <c r="V65" s="6"/>
     </row>
     <row r="66" spans="2:22" ht="17" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C66" s="20"/>
-      <c r="D66" s="21"/>
+      <c r="B66" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" s="28"/>
+      <c r="D66" s="29"/>
       <c r="E66" s="4"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
@@ -3811,23 +3799,23 @@
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
-      <c r="M66" s="74" t="s">
-        <v>32</v>
-      </c>
-      <c r="N66" s="67"/>
-      <c r="O66" s="63"/>
-      <c r="P66" s="63"/>
-      <c r="Q66" s="63"/>
-      <c r="R66" s="63"/>
-      <c r="S66" s="63"/>
-      <c r="T66" s="63"/>
-      <c r="U66" s="63"/>
+      <c r="M66" s="102" t="s">
+        <v>37</v>
+      </c>
+      <c r="N66" s="103"/>
+      <c r="O66" s="7"/>
+      <c r="P66" s="7"/>
+      <c r="Q66" s="7"/>
+      <c r="R66" s="7"/>
+      <c r="S66" s="7"/>
+      <c r="T66" s="7"/>
+      <c r="U66" s="7"/>
       <c r="V66" s="6"/>
     </row>
-    <row r="67" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B67" s="22"/>
-      <c r="C67" s="23"/>
-      <c r="D67" s="24"/>
+    <row r="67" spans="2:22" ht="17" x14ac:dyDescent="0.4">
+      <c r="B67" s="30"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="32"/>
       <c r="E67" s="4"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -3836,21 +3824,23 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
-      <c r="M67" s="5"/>
-      <c r="N67" s="63"/>
-      <c r="O67" s="63"/>
-      <c r="P67" s="63"/>
-      <c r="Q67" s="63"/>
-      <c r="R67" s="63"/>
-      <c r="S67" s="63"/>
-      <c r="T67" s="63"/>
-      <c r="U67" s="63"/>
+      <c r="M67" s="104" t="s">
+        <v>38</v>
+      </c>
+      <c r="N67" s="7"/>
+      <c r="O67" s="7"/>
+      <c r="P67" s="7"/>
+      <c r="Q67" s="7"/>
+      <c r="R67" s="7"/>
+      <c r="S67" s="7"/>
+      <c r="T67" s="7"/>
+      <c r="U67" s="7"/>
       <c r="V67" s="6"/>
     </row>
-    <row r="68" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B68" s="25"/>
-      <c r="C68" s="26"/>
-      <c r="D68" s="27"/>
+    <row r="68" spans="2:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B68" s="33"/>
+      <c r="C68" s="34"/>
+      <c r="D68" s="35"/>
       <c r="E68" s="4"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -3860,22 +3850,20 @@
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
       <c r="M68" s="5"/>
-      <c r="N68" s="91" t="s">
-        <v>33</v>
-      </c>
-      <c r="O68" s="92"/>
-      <c r="P68" s="92"/>
-      <c r="Q68" s="92"/>
-      <c r="R68" s="92"/>
-      <c r="S68" s="92"/>
-      <c r="T68" s="92"/>
-      <c r="U68" s="93"/>
+      <c r="N68" s="7"/>
+      <c r="O68" s="7"/>
+      <c r="P68" s="7"/>
+      <c r="Q68" s="7"/>
+      <c r="R68" s="7"/>
+      <c r="S68" s="7"/>
+      <c r="T68" s="7"/>
+      <c r="U68" s="7"/>
       <c r="V68" s="6"/>
     </row>
-    <row r="69" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="19"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="21"/>
+    <row r="69" spans="2:22" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B69" s="27"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="29"/>
       <c r="E69" s="4"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
@@ -3885,20 +3873,22 @@
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
       <c r="M69" s="5"/>
-      <c r="N69" s="94"/>
-      <c r="O69" s="95"/>
-      <c r="P69" s="95"/>
-      <c r="Q69" s="95"/>
-      <c r="R69" s="95"/>
-      <c r="S69" s="95"/>
-      <c r="T69" s="95"/>
-      <c r="U69" s="96"/>
+      <c r="N69" s="105" t="s">
+        <v>31</v>
+      </c>
+      <c r="O69" s="106"/>
+      <c r="P69" s="106"/>
+      <c r="Q69" s="106"/>
+      <c r="R69" s="106"/>
+      <c r="S69" s="106"/>
+      <c r="T69" s="106"/>
+      <c r="U69" s="107"/>
       <c r="V69" s="6"/>
     </row>
-    <row r="70" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B70" s="22"/>
-      <c r="C70" s="23"/>
-      <c r="D70" s="24"/>
+    <row r="70" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B70" s="30"/>
+      <c r="C70" s="31"/>
+      <c r="D70" s="32"/>
       <c r="E70" s="4"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
@@ -3908,20 +3898,20 @@
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
       <c r="M70" s="5"/>
-      <c r="N70" s="63"/>
-      <c r="O70" s="63"/>
-      <c r="P70" s="63"/>
-      <c r="Q70" s="63"/>
-      <c r="R70" s="63"/>
-      <c r="S70" s="63"/>
-      <c r="T70" s="63"/>
-      <c r="U70" s="63"/>
+      <c r="N70" s="108"/>
+      <c r="O70" s="109"/>
+      <c r="P70" s="109"/>
+      <c r="Q70" s="109"/>
+      <c r="R70" s="109"/>
+      <c r="S70" s="109"/>
+      <c r="T70" s="109"/>
+      <c r="U70" s="110"/>
       <c r="V70" s="6"/>
     </row>
-    <row r="71" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B71" s="25"/>
-      <c r="C71" s="26"/>
-      <c r="D71" s="27"/>
+    <row r="71" spans="2:22" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B71" s="33"/>
+      <c r="C71" s="34"/>
+      <c r="D71" s="35"/>
       <c r="E71" s="2"/>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
@@ -3930,22 +3920,24 @@
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
-      <c r="M71" s="64"/>
-      <c r="N71" s="65"/>
-      <c r="O71" s="65"/>
-      <c r="P71" s="65"/>
-      <c r="Q71" s="65"/>
-      <c r="R71" s="65"/>
-      <c r="S71" s="65"/>
-      <c r="T71" s="65"/>
-      <c r="U71" s="65"/>
-      <c r="V71" s="66"/>
+      <c r="M71" s="8"/>
+      <c r="N71" s="9"/>
+      <c r="O71" s="9"/>
+      <c r="P71" s="9"/>
+      <c r="Q71" s="9"/>
+      <c r="R71" s="9"/>
+      <c r="S71" s="9"/>
+      <c r="T71" s="9"/>
+      <c r="U71" s="9"/>
+      <c r="V71" s="10"/>
     </row>
     <row r="72" spans="2:22" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="54">
+  <mergeCells count="56">
+    <mergeCell ref="N69:U70"/>
+    <mergeCell ref="E28:L29"/>
+    <mergeCell ref="M28:V29"/>
     <mergeCell ref="M66:N66"/>
-    <mergeCell ref="N68:U69"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B12:D13"/>
     <mergeCell ref="B14:D15"/>
@@ -3958,15 +3950,6 @@
     <mergeCell ref="O34:P34"/>
     <mergeCell ref="R34:S34"/>
     <mergeCell ref="M59:O59"/>
-    <mergeCell ref="P59:R59"/>
-    <mergeCell ref="M61:O61"/>
-    <mergeCell ref="P61:R61"/>
-    <mergeCell ref="M63:N63"/>
-    <mergeCell ref="P63:R63"/>
-    <mergeCell ref="E28:L29"/>
-    <mergeCell ref="M28:V29"/>
-    <mergeCell ref="B60:D62"/>
-    <mergeCell ref="B63:D65"/>
     <mergeCell ref="B66:D68"/>
     <mergeCell ref="B39:D41"/>
     <mergeCell ref="M30:V32"/>
@@ -3976,6 +3959,13 @@
     <mergeCell ref="O38:S38"/>
     <mergeCell ref="O36:S36"/>
     <mergeCell ref="O40:S41"/>
+    <mergeCell ref="P61:R61"/>
+    <mergeCell ref="M63:N63"/>
+    <mergeCell ref="P63:R63"/>
+    <mergeCell ref="P59:R59"/>
+    <mergeCell ref="M61:O61"/>
+    <mergeCell ref="M64:N64"/>
+    <mergeCell ref="M65:N65"/>
     <mergeCell ref="B69:D71"/>
     <mergeCell ref="F31:H36"/>
     <mergeCell ref="F37:H37"/>
@@ -3990,6 +3980,8 @@
     <mergeCell ref="B28:D32"/>
     <mergeCell ref="B33:D35"/>
     <mergeCell ref="B36:D38"/>
+    <mergeCell ref="B60:D62"/>
+    <mergeCell ref="B63:D65"/>
     <mergeCell ref="B2:D7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>

</xml_diff>